<commit_message>
Update Shiny Add RiskFactorPlot for DefaultCurve
</commit_message>
<xml_diff>
--- a/src/data/bankA/rf_contracts.xlsx
+++ b/src/data/bankA/rf_contracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/bankA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80301D67-3100-2844-BC4B-1339B7B7AE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48F1FD8-10C9-7743-B428-4D2F7FBBF097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="500" windowWidth="22080" windowHeight="20500" xr2:uid="{1A9FC95E-9ECC-8D4D-827B-24BA29525206}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>rfType</t>
   </si>
@@ -80,9 +80,6 @@
     <t>tenor.5</t>
   </si>
   <si>
-    <t>YC_CTRS</t>
-  </si>
-  <si>
     <t>1Y</t>
   </si>
   <si>
@@ -96,6 +93,12 @@
   </si>
   <si>
     <t>15Y</t>
+  </si>
+  <si>
+    <t>YC_Default</t>
+  </si>
+  <si>
+    <t>YC_Shifted</t>
   </si>
 </sst>
 </file>
@@ -103,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -136,7 +139,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D4F580-6691-2A49-BB45-66ECF91A9EC2}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,39 +513,80 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <v>42736</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>0.01</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2">
         <v>0.02</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2">
         <v>0.03</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42736</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>0.01</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>0.02</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3">
+        <v>0.03</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>